<commit_message>
Updated graphs, lil reformatting
</commit_message>
<xml_diff>
--- a/results/results1_graph.xlsx
+++ b/results/results1_graph.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="1120" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="results1" sheetId="1" r:id="rId1"/>
@@ -140,63 +140,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Ideal Partition Numbers</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -392,11 +336,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="-2048673584"/>
-        <c:axId val="-2045073760"/>
+        <c:axId val="-2076308304"/>
+        <c:axId val="-2061615024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2048673584"/>
+        <c:axId val="-2076308304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -439,7 +383,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2045073760"/>
+        <c:crossAx val="-2061615024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -447,7 +391,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2045073760"/>
+        <c:axId val="-2061615024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -467,6 +411,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -497,7 +442,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2048673584"/>
+        <c:crossAx val="-2076308304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -550,12 +495,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1128,7 +1068,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
+      <xdr:colOff>723900</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>

</xml_diff>